<commit_message>
Run tests, get results, tweaks
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/activity_timeline.xlsx
+++ b/tests/integration_test_files/activity_timeline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/github/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAFB8F1D-E246-5A4B-8490-CAF8DEC38D80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10198DD7-6651-C246-887A-D114C318CDC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="6" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="760" yWindow="500" windowWidth="35400" windowHeight="18780" activeTab="9" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1156" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1161" uniqueCount="517">
   <si>
     <t>Screening</t>
   </si>
@@ -1618,6 +1618,18 @@
   </si>
   <si>
     <t>Extra</t>
+  </si>
+  <si>
+    <t>INSTANCE_100</t>
+  </si>
+  <si>
+    <t>TIMING_35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An extra timeline </t>
+  </si>
+  <si>
+    <t>From a scheduled activity instance</t>
   </si>
 </sst>
 </file>
@@ -2430,12 +2442,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{793CF704-5026-334C-9F38-E198AA4BC008}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D37" sqref="D37"/>
       <selection pane="topRight" activeCell="D37" sqref="D37"/>
       <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
-      <selection pane="bottomRight" activeCell="D1" sqref="D1:D1048576"/>
+      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2451,13 +2463,13 @@
         <v>83</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>265</v>
+        <v>512</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>270</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>377</v>
+        <v>513</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -2465,7 +2477,7 @@
         <v>85</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>266</v>
+        <v>515</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>26</v>
@@ -2476,7 +2488,7 @@
         <v>87</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>268</v>
+        <v>516</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>280</v>
@@ -2499,7 +2511,7 @@
         <v>333</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>378</v>
+        <v>334</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -2553,15 +2565,15 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D22D6280-6618-9149-96EE-53C1C0C7E8E9}">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView topLeftCell="A16" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10" style="34" customWidth="1"/>
+    <col min="1" max="1" width="13" style="34" customWidth="1"/>
     <col min="2" max="2" width="21.83203125" style="34" customWidth="1"/>
     <col min="3" max="3" width="22.1640625" style="34" customWidth="1"/>
     <col min="4" max="4" width="13.5" style="34" customWidth="1"/>
@@ -3400,6 +3412,26 @@
       <c r="H35" t="s">
         <v>356</v>
       </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>514</v>
+      </c>
+      <c r="B36"/>
+      <c r="C36"/>
+      <c r="D36" t="s">
+        <v>358</v>
+      </c>
+      <c r="E36" t="s">
+        <v>513</v>
+      </c>
+      <c r="F36" t="s">
+        <v>513</v>
+      </c>
+      <c r="G36" t="s">
+        <v>433</v>
+      </c>
+      <c r="H36"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -5966,8 +5998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136502A0-3DDE-CC47-9DA7-EB2F3073B24B}">
   <dimension ref="A1:P38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
       <selection pane="bottomRight" activeCell="I12" sqref="I12"/>

</xml_diff>